<commit_message>
Task 5, creating a scatter plot, is now completed
</commit_message>
<xml_diff>
--- a/assessment/iris_dataset.xlsx
+++ b/assessment/iris_dataset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="161">
   <si>
     <t xml:space="preserve">sepal_length,sepal_width,petal_length,petal_width,species</t>
   </si>
@@ -494,19 +494,29 @@
   </si>
   <si>
     <t xml:space="preserve">Variance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Median</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="#,##0.000"/>
     <numFmt numFmtId="167" formatCode="#,##0.00"/>
     <numFmt numFmtId="168" formatCode="0.00000"/>
     <numFmt numFmtId="169" formatCode="0.0000000"/>
+    <numFmt numFmtId="170" formatCode="0.00"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -539,17 +549,18 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FFC9211E"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -601,7 +612,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -622,6 +633,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -634,15 +649,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -655,6 +670,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FFC9211E"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -835,10 +910,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R119"/>
+  <dimension ref="A1:R1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B35" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R20" activeCellId="0" sqref="R20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -846,7 +921,7 @@
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.31"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="8" min="8" style="0" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="8" min="8" style="0" width="32.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="3.75"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="14" min="14" style="0" width="12.63"/>
   </cols>
@@ -3139,7 +3214,7 @@
       <c r="H48" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="I48" s="3" t="n">
+      <c r="I48" s="5" t="n">
         <v>5.7</v>
       </c>
       <c r="J48" s="3" t="n">
@@ -3368,51 +3443,51 @@
       <c r="B53" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C53" s="5" t="n">
+      <c r="C53" s="6" t="n">
         <f aca="false">AVERAGE(C$3:C$52)</f>
         <v>5.006</v>
       </c>
-      <c r="D53" s="6" t="n">
+      <c r="D53" s="7" t="n">
         <f aca="false">AVERAGE(D$3:D$52)</f>
         <v>3.418</v>
       </c>
-      <c r="E53" s="6" t="n">
+      <c r="E53" s="7" t="n">
         <f aca="false">AVERAGE(E$3:E$52)</f>
         <v>1.464</v>
       </c>
-      <c r="F53" s="6" t="n">
+      <c r="F53" s="7" t="n">
         <f aca="false">AVERAGE(F$3:F$52)</f>
         <v>0.244</v>
       </c>
-      <c r="I53" s="6" t="n">
+      <c r="I53" s="7" t="n">
         <f aca="false">AVERAGE(I$3:I$52)</f>
         <v>5.936</v>
       </c>
-      <c r="J53" s="6" t="n">
+      <c r="J53" s="7" t="n">
         <f aca="false">AVERAGE(J$3:J$52)</f>
         <v>2.77</v>
       </c>
-      <c r="K53" s="6" t="n">
+      <c r="K53" s="7" t="n">
         <f aca="false">AVERAGE(K$3:K$52)</f>
         <v>4.26</v>
       </c>
-      <c r="L53" s="6" t="n">
+      <c r="L53" s="7" t="n">
         <f aca="false">AVERAGE(L$3:L$52)</f>
         <v>1.326</v>
       </c>
-      <c r="O53" s="6" t="n">
+      <c r="O53" s="7" t="n">
         <f aca="false">AVERAGE(O$3:O$52)</f>
         <v>6.588</v>
       </c>
-      <c r="P53" s="6" t="n">
+      <c r="P53" s="7" t="n">
         <f aca="false">AVERAGE(P$3:P$52)</f>
         <v>2.974</v>
       </c>
-      <c r="Q53" s="6" t="n">
+      <c r="Q53" s="7" t="n">
         <f aca="false">AVERAGE(Q$3:Q$52)</f>
         <v>5.552</v>
       </c>
-      <c r="R53" s="6" t="n">
+      <c r="R53" s="7" t="n">
         <f aca="false">AVERAGE(R$3:R$52)</f>
         <v>2.026</v>
       </c>
@@ -3421,514 +3496,378 @@
       <c r="B54" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C54" s="7" t="n">
-        <f aca="false">STDEV(C$3:C$52)</f>
-        <v>0.352489687213451</v>
-      </c>
-      <c r="D54" s="7" t="n">
-        <f aca="false">STDEV(D$3:D$52)</f>
-        <v>0.381024397954691</v>
-      </c>
-      <c r="E54" s="7" t="n">
-        <f aca="false">STDEV(E$3:E$52)</f>
-        <v>0.173511159436446</v>
-      </c>
-      <c r="F54" s="7" t="n">
-        <f aca="false">STDEV(F$3:F$52)</f>
-        <v>0.107209503081678</v>
-      </c>
-      <c r="I54" s="7" t="n">
-        <f aca="false">STDEV(I$3:I$52)</f>
-        <v>0.516171147063864</v>
-      </c>
-      <c r="J54" s="7" t="n">
-        <f aca="false">STDEV(J$3:J$52)</f>
-        <v>0.313798323378412</v>
-      </c>
-      <c r="K54" s="7" t="n">
-        <f aca="false">STDEV(K$3:K$52)</f>
-        <v>0.469910977239958</v>
-      </c>
-      <c r="L54" s="7" t="n">
-        <f aca="false">STDEV(L$3:L$52)</f>
-        <v>0.197752680004544</v>
-      </c>
-      <c r="O54" s="7" t="n">
-        <f aca="false">STDEV(O$3:O$52)</f>
-        <v>0.635879593274432</v>
-      </c>
-      <c r="P54" s="7" t="n">
-        <f aca="false">STDEV(P$3:P$52)</f>
-        <v>0.322496638172638</v>
-      </c>
-      <c r="Q54" s="7" t="n">
-        <f aca="false">STDEV(Q$3:Q$52)</f>
-        <v>0.551894695663983</v>
-      </c>
-      <c r="R54" s="7" t="n">
-        <f aca="false">STDEV(R$3:R$52)</f>
-        <v>0.274650055636667</v>
+      <c r="C54" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(C$3:C$52)</f>
+        <v>0.348946987377739</v>
+      </c>
+      <c r="D54" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(D$3:D$52)</f>
+        <v>0.377194909827797</v>
+      </c>
+      <c r="E54" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(E$3:E$52)</f>
+        <v>0.171767284428671</v>
+      </c>
+      <c r="F54" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(F$3:F$52)</f>
+        <v>0.106131993291373</v>
+      </c>
+      <c r="G54" s="8"/>
+      <c r="I54" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(I$3:I$52)</f>
+        <v>0.510983365678375</v>
+      </c>
+      <c r="J54" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(J$3:J$52)</f>
+        <v>0.310644491340181</v>
+      </c>
+      <c r="K54" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(K$3:K$52)</f>
+        <v>0.46518813398452</v>
+      </c>
+      <c r="L54" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(L$3:L$52)</f>
+        <v>0.195765165440637</v>
+      </c>
+      <c r="M54" s="8"/>
+      <c r="O54" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(O$3:O$52)</f>
+        <v>0.629488681391493</v>
+      </c>
+      <c r="P54" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(P$3:P$52)</f>
+        <v>0.319255383666431</v>
+      </c>
+      <c r="Q54" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(Q$3:Q$52)</f>
+        <v>0.546347874526844</v>
+      </c>
+      <c r="R54" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(R$3:R$52)</f>
+        <v>0.27188968351153</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B55" s="8" t="s">
+      <c r="B55" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C55" s="9" t="n">
-        <f aca="false">VAR(C$3:C$52)</f>
-        <v>0.124248979591837</v>
-      </c>
-      <c r="D55" s="9" t="n">
-        <f aca="false">VAR(D$3:D$52)</f>
-        <v>0.145179591836735</v>
-      </c>
-      <c r="E55" s="9" t="n">
-        <f aca="false">VAR(E$3:E$52)</f>
-        <v>0.0301061224489796</v>
-      </c>
-      <c r="F55" s="9" t="n">
-        <f aca="false">VAR(F$3:F$52)</f>
-        <v>0.0114938775510204</v>
-      </c>
-      <c r="I55" s="9" t="n">
-        <f aca="false">VAR(I$3:I$52)</f>
-        <v>0.266432653061225</v>
-      </c>
-      <c r="J55" s="9" t="n">
-        <f aca="false">VAR(J$3:J$52)</f>
-        <v>0.0984693877551021</v>
-      </c>
-      <c r="K55" s="9" t="n">
-        <f aca="false">VAR(K$3:K$52)</f>
-        <v>0.220816326530612</v>
-      </c>
-      <c r="L55" s="9" t="n">
-        <f aca="false">VAR(L$3:L$52)</f>
-        <v>0.0391061224489796</v>
-      </c>
-      <c r="O55" s="9" t="n">
-        <f aca="false">VAR(O$3:O$52)</f>
-        <v>0.404342857142857</v>
-      </c>
-      <c r="P55" s="9" t="n">
-        <f aca="false">VAR(P$3:P$52)</f>
-        <v>0.104004081632653</v>
-      </c>
-      <c r="Q55" s="9" t="n">
-        <f aca="false">VAR(Q$3:Q$52)</f>
-        <v>0.304587755102041</v>
-      </c>
-      <c r="R55" s="9" t="n">
-        <f aca="false">VAR(R$3:R$52)</f>
-        <v>0.0754326530612245</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B69" s="0" t="n">
+      <c r="C55" s="10" t="n">
+        <f aca="false">_xlfn.VAR.P(C$3:C$52)</f>
+        <v>0.121764</v>
+      </c>
+      <c r="D55" s="10" t="n">
+        <f aca="false">_xlfn.VAR.P(D$3:D$52)</f>
+        <v>0.142276</v>
+      </c>
+      <c r="E55" s="10" t="n">
+        <f aca="false">_xlfn.VAR.P(E$3:E$52)</f>
+        <v>0.029504</v>
+      </c>
+      <c r="F55" s="10" t="n">
+        <f aca="false">_xlfn.VAR.P(F$3:F$52)</f>
+        <v>0.011264</v>
+      </c>
+      <c r="G55" s="10"/>
+      <c r="I55" s="10" t="n">
+        <f aca="false">_xlfn.VAR.P(I$3:I$52)</f>
+        <v>0.261104</v>
+      </c>
+      <c r="J55" s="10" t="n">
+        <f aca="false">_xlfn.VAR.P(J$3:J$52)</f>
+        <v>0.0965000000000001</v>
+      </c>
+      <c r="K55" s="10" t="n">
+        <f aca="false">_xlfn.VAR.P(K$3:K$52)</f>
+        <v>0.2164</v>
+      </c>
+      <c r="L55" s="10" t="n">
+        <f aca="false">_xlfn.VAR.P(L$3:L$52)</f>
+        <v>0.038324</v>
+      </c>
+      <c r="M55" s="10"/>
+      <c r="O55" s="10" t="n">
+        <f aca="false">_xlfn.VAR.P(O$3:O$52)</f>
+        <v>0.396256</v>
+      </c>
+      <c r="P55" s="10" t="n">
+        <f aca="false">_xlfn.VAR.P(P$3:P$52)</f>
+        <v>0.101924</v>
+      </c>
+      <c r="Q55" s="10" t="n">
+        <f aca="false">_xlfn.VAR.P(Q$3:Q$52)</f>
+        <v>0.298496</v>
+      </c>
+      <c r="R55" s="10" t="n">
+        <f aca="false">_xlfn.VAR.P(R$3:R$52)</f>
+        <v>0.073924</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B56" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="C56" s="11" t="n">
+        <f aca="false">MEDIAN(C3:C52)</f>
+        <v>5</v>
+      </c>
+      <c r="D56" s="11" t="n">
+        <f aca="false">MEDIAN(D3:D52)</f>
+        <v>3.4</v>
+      </c>
+      <c r="E56" s="11" t="n">
+        <f aca="false">MEDIAN(E3:E52)</f>
+        <v>1.5</v>
+      </c>
+      <c r="F56" s="11" t="n">
+        <f aca="false">MEDIAN(F3:F52)</f>
+        <v>0.2</v>
+      </c>
+      <c r="I56" s="11" t="n">
+        <f aca="false">MEDIAN(I3:I52)</f>
+        <v>5.9</v>
+      </c>
+      <c r="J56" s="11" t="n">
+        <f aca="false">MEDIAN(J3:J52)</f>
+        <v>2.8</v>
+      </c>
+      <c r="K56" s="11" t="n">
+        <f aca="false">MEDIAN(K3:K52)</f>
+        <v>4.35</v>
+      </c>
+      <c r="L56" s="11" t="n">
+        <f aca="false">MEDIAN(L3:L52)</f>
+        <v>1.3</v>
+      </c>
+      <c r="O56" s="11" t="n">
+        <f aca="false">MEDIAN(O3:O52)</f>
+        <v>6.5</v>
+      </c>
+      <c r="P56" s="11" t="n">
+        <f aca="false">MEDIAN(P3:P52)</f>
+        <v>3</v>
+      </c>
+      <c r="Q56" s="11" t="n">
+        <f aca="false">MEDIAN(Q3:Q52)</f>
+        <v>5.55</v>
+      </c>
+      <c r="R56" s="11" t="n">
+        <f aca="false">MEDIAN(R3:R52)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B57" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <f aca="false">MAX(C3:C52)</f>
+        <v>5.8</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <f aca="false">MAX(D3:D52)</f>
+        <v>4.4</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <f aca="false">MAX(E3:E52)</f>
+        <v>1.9</v>
+      </c>
+      <c r="F57" s="0" t="n">
+        <f aca="false">MAX(F3:F52)</f>
+        <v>0.6</v>
+      </c>
+      <c r="I57" s="0" t="n">
+        <f aca="false">MAX(I3:I52)</f>
+        <v>7</v>
+      </c>
+      <c r="J57" s="0" t="n">
+        <f aca="false">MAX(J3:J52)</f>
+        <v>3.4</v>
+      </c>
+      <c r="K57" s="0" t="n">
+        <f aca="false">MAX(K3:K52)</f>
         <v>5.1</v>
       </c>
-      <c r="C69" s="2" t="n">
-        <v>5.1</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B70" s="0" t="n">
+      <c r="L57" s="0" t="n">
+        <f aca="false">MAX(L3:L52)</f>
+        <v>1.8</v>
+      </c>
+      <c r="O57" s="0" t="n">
+        <f aca="false">MAX(O3:O52)</f>
+        <v>7.9</v>
+      </c>
+      <c r="P57" s="0" t="n">
+        <f aca="false">MAX(P3:P52)</f>
+        <v>3.8</v>
+      </c>
+      <c r="Q57" s="0" t="n">
+        <f aca="false">MAX(Q3:Q52)</f>
+        <v>6.9</v>
+      </c>
+      <c r="R57" s="0" t="n">
+        <f aca="false">MAX(R3:R52)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B58" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <f aca="false">MIN(C3:C52)</f>
+        <v>4.3</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <f aca="false">MIN(D3:D52)</f>
+        <v>2.3</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <f aca="false">MIN(E3:E52)</f>
+        <v>1</v>
+      </c>
+      <c r="F58" s="0" t="n">
+        <f aca="false">MIN(F3:F52)</f>
+        <v>0.1</v>
+      </c>
+      <c r="I58" s="0" t="n">
+        <f aca="false">MIN(I3:I52)</f>
         <v>4.9</v>
       </c>
-      <c r="C70" s="2" t="n">
+      <c r="J58" s="0" t="n">
+        <f aca="false">MIN(J3:J52)</f>
+        <v>2</v>
+      </c>
+      <c r="K58" s="0" t="n">
+        <f aca="false">MIN(K3:K52)</f>
+        <v>3</v>
+      </c>
+      <c r="L58" s="0" t="n">
+        <f aca="false">MIN(L3:L52)</f>
+        <v>1</v>
+      </c>
+      <c r="O58" s="0" t="n">
+        <f aca="false">MIN(O3:O52)</f>
         <v>4.9</v>
       </c>
-    </row>
-    <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B71" s="0" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="C71" s="3" t="n">
-        <v>4.7</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B72" s="0" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="C72" s="3" t="n">
-        <v>4.6</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B73" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C73" s="3" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B74" s="0" t="n">
-        <v>5.4</v>
-      </c>
-      <c r="C74" s="3" t="n">
-        <v>5.4</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B75" s="0" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="C75" s="3" t="n">
-        <v>4.6</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B76" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C76" s="3" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B77" s="0" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="C77" s="3" t="n">
-        <v>4.4</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B78" s="0" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="C78" s="3" t="n">
-        <v>4.9</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B79" s="0" t="n">
-        <v>5.4</v>
-      </c>
-      <c r="C79" s="3" t="n">
-        <v>5.4</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B80" s="10" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="C80" s="3" t="n">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B81" s="10" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="C81" s="3" t="n">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B82" s="0" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="C82" s="3" t="n">
-        <v>4.3</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B83" s="0" t="n">
-        <v>5.8</v>
-      </c>
-      <c r="C83" s="3" t="n">
-        <v>5.8</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B84" s="10" t="n">
-        <v>5.7</v>
-      </c>
-      <c r="C84" s="3" t="n">
-        <v>5.7</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B85" s="0" t="n">
-        <v>5.4</v>
-      </c>
-      <c r="C85" s="3" t="n">
-        <v>5.4</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B86" s="0" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="C86" s="3" t="n">
-        <v>5.1</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B87" s="10" t="n">
-        <v>5.7</v>
-      </c>
-      <c r="C87" s="3" t="n">
-        <v>5.7</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B88" s="10" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="C88" s="3" t="n">
-        <v>5.1</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B89" s="10" t="n">
-        <v>5.4</v>
-      </c>
-      <c r="C89" s="3" t="n">
-        <v>5.4</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B90" s="10" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="C90" s="3" t="n">
-        <v>5.1</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B91" s="0" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="C91" s="3" t="n">
-        <v>4.6</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B92" s="0" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="C92" s="3" t="n">
-        <v>5.1</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B93" s="0" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="C93" s="3" t="n">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B94" s="10" t="n">
-        <v>5</v>
-      </c>
-      <c r="C94" s="3" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B95" s="10" t="n">
-        <v>5</v>
-      </c>
-      <c r="C95" s="3" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B96" s="10" t="n">
-        <v>5.2</v>
-      </c>
-      <c r="C96" s="3" t="n">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B97" s="0" t="n">
-        <v>5.2</v>
-      </c>
-      <c r="C97" s="3" t="n">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B98" s="0" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="C98" s="3" t="n">
-        <v>4.7</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B99" s="0" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="C99" s="3" t="n">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B100" s="0" t="n">
-        <v>5.4</v>
-      </c>
-      <c r="C100" s="3" t="n">
-        <v>5.4</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B101" s="0" t="n">
-        <v>5.2</v>
-      </c>
-      <c r="C101" s="3" t="n">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B102" s="0" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="C102" s="3" t="n">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B103" s="10" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="C103" s="3" t="n">
-        <v>4.9</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B104" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C104" s="3" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B105" s="0" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="C105" s="3" t="n">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B106" s="0" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="C106" s="3" t="n">
-        <v>4.9</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B107" s="0" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="C107" s="3" t="n">
-        <v>4.4</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B108" s="0" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="C108" s="3" t="n">
-        <v>5.1</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B109" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C109" s="3" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B110" s="0" t="n">
+      <c r="P58" s="0" t="n">
+        <f aca="false">MIN(P3:P52)</f>
+        <v>2.2</v>
+      </c>
+      <c r="Q58" s="0" t="n">
+        <f aca="false">MIN(Q3:Q52)</f>
         <v>4.5</v>
       </c>
-      <c r="C110" s="3" t="n">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B111" s="0" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="C111" s="3" t="n">
-        <v>4.4</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B112" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C112" s="3" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B113" s="0" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="C113" s="3" t="n">
-        <v>5.1</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B114" s="0" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="C114" s="3" t="n">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B115" s="10" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="C115" s="3" t="n">
-        <v>5.1</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B116" s="0" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="C116" s="3" t="n">
-        <v>4.6</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B117" s="0" t="n">
-        <v>5.3</v>
-      </c>
-      <c r="C117" s="3" t="n">
-        <v>5.3</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B118" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C118" s="3" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B119" s="0" t="n">
-        <f aca="false">AVERAGE(B69:B118)</f>
-        <v>5.006</v>
-      </c>
-    </row>
+      <c r="R58" s="0" t="n">
+        <f aca="false">MIN(R3:R52)</f>
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="1048470" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048471" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048472" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048473" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048474" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048475" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048476" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048477" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048478" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048479" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048480" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048481" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048482" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048483" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048484" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048485" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048486" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048487" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048488" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048489" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048490" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048491" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048492" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048493" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048494" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048495" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048496" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048497" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048498" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048499" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048500" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048501" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048502" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048503" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048504" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048505" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048506" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048507" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048508" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048509" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048510" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>